<commit_message>
Fix crash Misc refactors
</commit_message>
<xml_diff>
--- a/Pricelist.xlsx
+++ b/Pricelist.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="152511" fullCalcOnLoad="1"/>
@@ -482,7 +482,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0,46€</t>
+          <t>0,59€</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -507,7 +507,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1,35€</t>
+          <t>0,32€</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -532,7 +532,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1,78€</t>
+          <t>2,10€</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -557,7 +557,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0,38€</t>
+          <t>1,44€</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -582,12 +582,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0,93€</t>
+          <t>35,56€</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Psychonauts in the Rhombus of Ruin PC</t>
+          <t>Psychonauts 2 PC</t>
         </is>
       </c>
     </row>
@@ -607,7 +607,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0,73€</t>
+          <t>0,82€</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -632,7 +632,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0,39€</t>
+          <t>0,79€</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -657,7 +657,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2,46€</t>
+          <t>1,30€</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -682,7 +682,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0,28€</t>
+          <t>0,19€</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -707,7 +707,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0,30€</t>
+          <t>0,42€</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -732,7 +732,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0,82€</t>
+          <t>1,06€</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -757,7 +757,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1,35€</t>
+          <t>2,53€</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -782,7 +782,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0,39€</t>
+          <t>0,86€</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -807,7 +807,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0,35€</t>
+          <t>0,55€</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -832,7 +832,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0,60€</t>
+          <t>0,81€</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -857,7 +857,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0,93€</t>
+          <t>1,32€</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -882,7 +882,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0,31€</t>
+          <t>0,22€</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -907,7 +907,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1,19€</t>
+          <t>1,31€</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -932,7 +932,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0,43€</t>
+          <t>0,76€</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -955,12 +955,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0,43€</t>
+          <t>5,47€</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Earth 2140 PC</t>
+          <t>Anno 1404 - History Edition PC</t>
         </is>
       </c>
     </row>
@@ -980,7 +980,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1,79€</t>
+          <t>2,68€</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1,26€</t>
+          <t>2,99€</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1,86€</t>
+          <t>2,04€</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1055,7 +1055,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1,24€</t>
+          <t>0,87€</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1080,7 +1080,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1,24€</t>
+          <t>0,87€</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1105,7 +1105,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2,99€</t>
+          <t>3,03€</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1130,7 +1130,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1,34€</t>
+          <t>0,98€</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0,47€</t>
+          <t>0,44€</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1180,7 +1180,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>0,60€</t>
+          <t>0,93€</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1,02€</t>
+          <t>0,97€</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1230,7 +1230,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>0,99€</t>
+          <t>0,84€</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1255,12 +1255,12 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>5,97€</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Duke Nukem: Manhattan Project PC</t>
         </is>
       </c>
     </row>
@@ -1280,7 +1280,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0,87€</t>
+          <t>0,50€</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1305,12 +1305,12 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0,39€</t>
+          <t>8,19€</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Hush Hush - Unlimited Survival Horror PC</t>
+          <t>蜀山幻剑录 Sword of Shushan PC</t>
         </is>
       </c>
     </row>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0,94€</t>
+          <t>0,97€</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1355,7 +1355,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>1,99€</t>
+          <t>9,99€</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1405,7 +1405,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2,33€</t>
+          <t>1,49€</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -1430,7 +1430,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1,38€</t>
+          <t>0,98€</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1455,7 +1455,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>0,49€</t>
+          <t>0,40€</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1480,7 +1480,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>0,67€</t>
+          <t>3,59€</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1530,7 +1530,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0,81€</t>
+          <t>2,39€</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -1555,7 +1555,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1,43€</t>
+          <t>1,47€</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>0,44€</t>
+          <t>0,71€</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -1605,7 +1605,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1,82€</t>
+          <t>0,73€</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -1630,7 +1630,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>0,39€</t>
+          <t>1,69€</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -1655,7 +1655,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>6,24€</t>
+          <t>5,31€</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -1680,12 +1680,12 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>0,98€</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Spark Rising PC</t>
         </is>
       </c>
     </row>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1,08€</t>
+          <t>0,30€</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -1730,7 +1730,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2,49€</t>
+          <t>8,49€</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -1755,7 +1755,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1,99€</t>
+          <t>1,50€</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -1780,7 +1780,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>0,60€</t>
+          <t>2,48€</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -1805,7 +1805,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1,64€</t>
+          <t>3,35€</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -1830,7 +1830,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1,09€</t>
+          <t>0,84€</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -1855,12 +1855,12 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>3,44€</t>
+          <t>11,01€</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Wild Season PC</t>
+          <t>Tom Clancy's Ghost Recon Wildlands - Season Pass Year 1 PC</t>
         </is>
       </c>
     </row>
@@ -1880,7 +1880,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>0,93€</t>
+          <t>0,75€</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -1905,7 +1905,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>0,34€</t>
+          <t>0,30€</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -1930,7 +1930,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>0,34€</t>
+          <t>0,25€</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -1955,7 +1955,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>0,34€</t>
+          <t>0,36€</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -1980,7 +1980,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>0,34€</t>
+          <t>0,25€</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -2010,7 +2010,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>0,64€</t>
+          <t>0,25€</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -2035,7 +2035,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>0,39€</t>
+          <t>0,15€</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -2060,7 +2060,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>0,53€</t>
+          <t>0,79€</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -2085,7 +2085,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>0,70€</t>
+          <t>1,00€</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -2115,12 +2115,12 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>0,51€</t>
+          <t>19,79€</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>World War II: Panzer Claws PC</t>
+          <t>Call of Duty: WWII PC</t>
         </is>
       </c>
     </row>
@@ -2140,7 +2140,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>0,54€</t>
+          <t>0,25€</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -2165,7 +2165,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>0,64€</t>
+          <t>0,15€</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -2190,7 +2190,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>4,49€</t>
+          <t>4,30€</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -2215,12 +2215,12 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>6,29€</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>The Incredible Adventures of Van Helsing II + 2 DLC PC</t>
         </is>
       </c>
     </row>
@@ -2240,7 +2240,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1,22€</t>
+          <t>7,63€</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>0,97€</t>
+          <t>0,96€</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -2290,7 +2290,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>0,40€</t>
+          <t>0,18€</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -2315,7 +2315,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>0,48€</t>
+          <t>0,18€</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -2345,7 +2345,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1,81€</t>
+          <t>0,50€</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -2375,7 +2375,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1,17€</t>
+          <t>0,97€</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -2400,7 +2400,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>1,72€</t>
+          <t>1,74€</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -2430,7 +2430,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>1,74€</t>
+          <t>1,75€</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -2460,7 +2460,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>1,35€</t>
+          <t>0,55€</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -2490,7 +2490,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>1,32€</t>
+          <t>1,78€</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -2515,7 +2515,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>0,41€</t>
+          <t>0,73€</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>0,72€</t>
+          <t>0,36€</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -2565,12 +2565,12 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>3,24€</t>
+          <t>5,83€</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>仙劍奇俠傳六 (Chinese Paladin：Sword and Fairy 6) PC</t>
+          <t>Chinese Paladin：Sword and Fairy 6 PC</t>
         </is>
       </c>
     </row>
@@ -2590,12 +2590,12 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>4,19€</t>
+          <t>3,24€</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>軒轅劍外傳穹之扉(The Gate of Firmament) PC</t>
+          <t>Xuan-Yuan Sword: The Gate of Firmament PC</t>
         </is>
       </c>
     </row>
@@ -2620,7 +2620,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>3,99€</t>
+          <t>4,85€</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -2645,7 +2645,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>1,98€</t>
+          <t>1,94€</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -2670,7 +2670,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>0,59€</t>
+          <t>0,43€</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -2695,7 +2695,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>0,59€</t>
+          <t>0,45€</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -2720,7 +2720,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>0,99€</t>
+          <t>1,16€</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -2745,7 +2745,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>2,99€</t>
+          <t>2,39€</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -2770,7 +2770,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>0,50€</t>
+          <t>0,19€</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -2795,7 +2795,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>0,80€</t>
+          <t>0,56€</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -2820,7 +2820,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>0,35€</t>
+          <t>0,24€</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -2845,7 +2845,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>0,62€</t>
+          <t>0,59€</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -2870,7 +2870,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>0,35€</t>
+          <t>0,29€</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -2895,7 +2895,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>0,98€</t>
+          <t>0,42€</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -2920,7 +2920,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>0,38€</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -2945,7 +2945,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>0,35€</t>
+          <t>0,28€</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -2970,7 +2970,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>0,47€</t>
+          <t>1,59€</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -2995,7 +2995,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>1,43€</t>
+          <t>0,83€</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -3020,7 +3020,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>0,83€</t>
+          <t>0,92€</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -3045,12 +3045,12 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>0,89€</t>
+          <t>19,99€</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Space Hack PC</t>
+          <t>Yolo Space Hacker PC</t>
         </is>
       </c>
     </row>
@@ -3075,7 +3075,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>2,49€</t>
+          <t>4,03€</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -3100,7 +3100,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>3,43€</t>
+          <t>3,52€</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -3125,7 +3125,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>1,66€</t>
+          <t>1,29€</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -3150,7 +3150,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>0,87€</t>
+          <t>0,98€</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -3180,7 +3180,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>0,52€</t>
+          <t>0,26€</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>1,74€</t>
+          <t>1,39€</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -3235,12 +3235,12 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>0,57€</t>
+          <t>4,89€</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Hero of the Kingdom III PC</t>
+          <t>Hero of the Kingdom: The Lost Tales 2 PC</t>
         </is>
       </c>
     </row>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>0,40€</t>
+          <t>2,34€</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -3310,7 +3310,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>0,92€</t>
+          <t>1,08€</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -3335,7 +3335,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>2,25€</t>
+          <t>5,07€</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -3365,7 +3365,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>0,57€</t>
+          <t>0,31€</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -3395,7 +3395,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>1,43€</t>
+          <t>1,25€</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -3420,7 +3420,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>0,63€</t>
+          <t>0,65€</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -3445,7 +3445,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>1,89€</t>
+          <t>2,34€</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -3470,12 +3470,12 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>3,29€</t>
+          <t>1,98€</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Company of Heroes 2 - Ardennes Assault PC</t>
+          <t>Company of Heroes 2 PC</t>
         </is>
       </c>
     </row>
@@ -3495,7 +3495,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>1,55€</t>
+          <t>2,90€</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -3520,7 +3520,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>2,02€</t>
+          <t>1,82€</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -3545,12 +3545,12 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>27,02€</t>
+          <t>3,73€</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Team Sonic Racing PC</t>
+          <t>Sonic Mania PC</t>
         </is>
       </c>
     </row>
@@ -3570,7 +3570,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>0,31€</t>
+          <t>0,27€</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -3595,7 +3595,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>0,94€</t>
+          <t>1,25€</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -3620,7 +3620,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>9,20€</t>
+          <t>10,25€</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -3645,7 +3645,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>14,88€</t>
+          <t>16,79€</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -3695,7 +3695,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>0,55€</t>
+          <t>0,44€</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -3720,7 +3720,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>8,65€</t>
+          <t>6,06€</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -3745,7 +3745,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>1,65€</t>
+          <t>0,76€</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -3770,7 +3770,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>0,54€</t>
+          <t>0,37€</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -3795,12 +3795,12 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>7,99€</t>
+          <t>2,38€</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Surviving Mars: First Colony Edition PC</t>
+          <t>Surviving Mars PC</t>
         </is>
       </c>
     </row>
@@ -3820,7 +3820,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>4,94€</t>
+          <t>5,44€</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -3845,7 +3845,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>0,40€</t>
+          <t>0,59€</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -3870,7 +3870,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>0,15€</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -3895,12 +3895,12 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>0,44€</t>
+          <t>1,90€</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>GoNNER (GONNER2 Out Now!) PC</t>
+          <t>GONNER2 PC</t>
         </is>
       </c>
     </row>
@@ -3920,7 +3920,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>0,99€</t>
+          <t>1,83€</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>0,59€</t>
+          <t>0,31€</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -3970,7 +3970,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>0,90€</t>
+          <t>1,80€</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -3995,7 +3995,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>3,39€</t>
+          <t>3,83€</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -4020,7 +4020,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>9,99€</t>
+          <t>10,39€</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -4045,7 +4045,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>1,71€</t>
+          <t>3,07€</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -4070,7 +4070,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>0,41€</t>
+          <t>0,36€</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -4095,12 +4095,12 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>0,30€</t>
+          <t>11,48€</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>All You Can Eat PC</t>
+          <t>Overcooked! All You Can Eat PC</t>
         </is>
       </c>
     </row>
@@ -4145,7 +4145,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>0,40€</t>
+          <t>0,45€</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -4170,7 +4170,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>0,65€</t>
+          <t>0,50€</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -4195,7 +4195,7 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>0,45€</t>
+          <t>0,30€</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -4220,12 +4220,12 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>9,99€</t>
+          <t>0,28€</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>Vertiginous Golf - Gold Pack Upgrade PC</t>
+          <t>Vertiginous Golf PC</t>
         </is>
       </c>
     </row>
@@ -4245,7 +4245,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>0,54€</t>
+          <t>0,50€</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -4270,7 +4270,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>0,31€</t>
+          <t>0,39€</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -4295,7 +4295,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>0,41€</t>
+          <t>0,25€</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -4320,12 +4320,12 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>0,35€</t>
+          <t>5,98€</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>Realpolitiks PC</t>
+          <t>Realpolitiks II PC</t>
         </is>
       </c>
     </row>
@@ -4345,7 +4345,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>31,52€</t>
+          <t>13,62€</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -4370,12 +4370,12 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>4,69€</t>
+          <t>16,79€</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>Bright Memory PC</t>
+          <t>Bright Memory: Infinite PC</t>
         </is>
       </c>
     </row>
@@ -4395,7 +4395,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>0,30€</t>
+          <t>0,39€</t>
         </is>
       </c>
       <c r="F157" s="10" t="inlineStr">
@@ -4420,7 +4420,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>1,88€</t>
+          <t>2,64€</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -4445,7 +4445,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>0,52€</t>
+          <t>0,48€</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -4470,7 +4470,7 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>0,80€</t>
+          <t>0,64€</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -4495,7 +4495,7 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>0,35€</t>
+          <t>0,28€</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -4545,7 +4545,7 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>0,44€</t>
+          <t>0,58€</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -4570,7 +4570,7 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>0,44€</t>
+          <t>0,35€</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -4595,7 +4595,7 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>5,83€</t>
+          <t>7,49€</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -4620,12 +4620,12 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>0,75€</t>
+          <t>10,34€</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>Overload PC</t>
+          <t>NEEDY STREAMER OVERLOAD PC</t>
         </is>
       </c>
     </row>
@@ -4646,7 +4646,7 @@
       <c r="D167" s="10" t="n"/>
       <c r="E167" t="inlineStr">
         <is>
-          <t>0,35€</t>
+          <t>0,68€</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -4671,7 +4671,7 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>0,59€</t>
+          <t>0,55€</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -4696,7 +4696,7 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>2,19€</t>
+          <t>2,14€</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -4746,7 +4746,7 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>0,67€</t>
+          <t>2,42€</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -4771,7 +4771,7 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>0,90€</t>
+          <t>1,26€</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -4796,7 +4796,7 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>45,13€</t>
+          <t>59,99€</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">

</xml_diff>